<commit_message>
Updated all the makefiles with a benchmark entry
</commit_message>
<xml_diff>
--- a/examples_timings.xlsx
+++ b/examples_timings.xlsx
@@ -25,9 +25,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="1" count="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="2" count="2">
   <si>
     <t>Intel core i9-9900K@3.6GHz</t>
+  </si>
+  <si>
+    <t>7.0.1 (develop)</t>
   </si>
 </sst>
 </file>
@@ -97,17 +100,17 @@
   <sheetPr>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:L7"/>
+  <dimension ref="A1:L9"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="1">
-      <selection activeCell="H8" sqref="H8"/>
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
     <col min="1" max="1" style="0" width="10.999338942307693" bestFit="1" customWidth="1"/>
     <col min="2" max="2" style="0" width="16.28473557692308" customWidth="1"/>
-    <col min="3" max="256" style="0" width="9.142307692307693"/>
+    <col min="3" max="16384" style="0" width="9.142307692307693"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12">
@@ -243,6 +246,62 @@
       <c r="L7" t="inlineStr">
         <is>
           <t>I was expecting this to be a lot quicker!</t>
+        </is>
+      </c>
+    </row>
+    <row r="8" spans="1:12">
+      <c r="A8" s="1">
+        <v>44498</v>
+      </c>
+      <c r="B8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C8">
+        <v>589.29999999999995</v>
+      </c>
+      <c r="D8">
+        <v>20.829999999999998</v>
+      </c>
+      <c r="E8">
+        <v>262</v>
+      </c>
+      <c r="F8">
+        <v>232.59</v>
+      </c>
+      <c r="H8" t="s">
+        <v>0</v>
+      </c>
+      <c r="L8" t="inlineStr">
+        <is>
+          <t>A bit better.</t>
+        </is>
+      </c>
+    </row>
+    <row r="9" spans="1:12">
+      <c r="A9" s="1">
+        <v>44498</v>
+      </c>
+      <c r="B9" t="s">
+        <v>1</v>
+      </c>
+      <c r="C9">
+        <v>469.01999999999998</v>
+      </c>
+      <c r="D9">
+        <v>19.469999999999999</v>
+      </c>
+      <c r="E9">
+        <v>453</v>
+      </c>
+      <c r="F9">
+        <v>107.65000000000001</v>
+      </c>
+      <c r="H9" t="s">
+        <v>0</v>
+      </c>
+      <c r="L9" t="inlineStr">
+        <is>
+          <t>Removed excel checking</t>
         </is>
       </c>
     </row>
@@ -271,8 +330,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
-    <col min="1" max="1" style="0" width="9.142307692307693"/>
-    <col min="2" max="256" style="0" width="9.142307692307693"/>
+    <col min="1" max="16384" style="0" width="9.142307692307693"/>
   </cols>
   <sheetData/>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" selectLockedCells="1" sort="0" autoFilter="0" pivotTables="0" selectUnlockedCells="1"/>
@@ -299,8 +357,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
-    <col min="1" max="1" style="0" width="9.142307692307693"/>
-    <col min="2" max="256" style="0" width="9.142307692307693"/>
+    <col min="1" max="16384" style="0" width="9.142307692307693"/>
   </cols>
   <sheetData/>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" selectLockedCells="1" sort="0" autoFilter="0" pivotTables="0" selectUnlockedCells="1"/>

</xml_diff>